<commit_message>
PROS-11454 - CCJP setup and template update
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -63,6 +63,12 @@
   </si>
   <si>
     <t xml:space="preserve">Include POSM</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_1_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_1_value</t>
   </si>
   <si>
     <t xml:space="preserve">Facings SOS</t>
@@ -205,11 +211,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -304,7 +310,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -315,33 +321,37 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:65536"/>
+  <dimension ref="1:3"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J2" activeCellId="0" sqref="J2"/>
+      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="20.8866396761134"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="28.9230769230769"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="13.9271255060729"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="20.995951417004"/>
-    <col collapsed="false" hidden="false" max="9" min="8" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="32.9919028340081"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="28.4939271255061"/>
-    <col collapsed="false" hidden="false" max="1014" min="12" style="1" width="8.78542510121457"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="8.78542510121457"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0404858299595"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.412955465587"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8502024291498"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1740890688259"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.9757085020243"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.497975708502"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.4372469635628"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.2874493927126"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.5546558704453"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6518218623482"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.9028340080972"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.0242914979757"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="22.5384615384615"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.2226720647773"/>
+    <col collapsed="false" hidden="false" max="1014" min="15" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="46" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" s="4" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -378,6 +388,16 @@
       <c r="L1" s="3" t="s">
         <v>11</v>
       </c>
+      <c r="M1" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="3"/>
+      <c r="P1" s="3"/>
+      <c r="Q1" s="3"/>
+      <c r="R1" s="3"/>
       <c r="AMA1" s="0"/>
       <c r="AMB1" s="0"/>
       <c r="AMC1" s="0"/>
@@ -389,34 +409,34 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="40.7" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" s="5" customFormat="true" ht="148.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="5" t="s">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B2" s="6"/>
       <c r="C2" s="6" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="F2" s="7" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="G2" s="8" t="s">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="7" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" s="7"/>
       <c r="L2" s="7" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="AMA2" s="0"/>
       <c r="AMB2" s="0"/>
@@ -429,23 +449,22 @@
       <c r="AMI2" s="0"/>
       <c r="AMJ2" s="0"/>
     </row>
-    <row r="3" customFormat="false" ht="29" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="5"/>
       <c r="C3" s="6"/>
       <c r="D3" s="7" t="s">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="F3" s="5"/>
       <c r="G3" s="8"/>
       <c r="J3" s="7"/>
       <c r="L3" s="5" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
PROS-11454 CCJP KPI development bug fix when FSOS is empty
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -65,32 +65,91 @@
     <t xml:space="preserve">Include POSM</t>
   </si>
   <si>
+    <t xml:space="preserve">additional_kpi_attributes</t>
+  </si>
+  <si>
     <t xml:space="preserve">store_attr_1_name</t>
   </si>
   <si>
     <t xml:space="preserve">store_attr_1_value</t>
   </si>
   <si>
+    <t xml:space="preserve">store_attr_2_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_2_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_3_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_3_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_4_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_4_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_5_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_5_value</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_6_name</t>
+  </si>
+  <si>
+    <t xml:space="preserve">store_attr_6_value</t>
+  </si>
+  <si>
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
     <t xml:space="preserve">Cold Teiban, Ambient Teiban</t>
   </si>
   <si>
-    <t xml:space="preserve">Include </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Include</t>
+    <t xml:space="preserve">include </t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude</t>
   </si>
   <si>
     <t xml:space="preserve">Other, SSD, Coffee, Fruit Juice, 
 NS Tea, Black Tea, Sports, Energy, Water, Vegetable Juice</t>
   </si>
   <si>
-    <t xml:space="preserve">Exclude</t>
+    <t xml:space="preserve">address_city</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tokyo</t>
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_POC_COUNT_BY_STORE_AREA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_POC_SCORE_BY_TARGET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_RED_SCORE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{'poc_weightage':0.42,
+'dist_weightage':0.42,
+'sovi_weightage':0.16}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_UNIQUE_DIST_OWN_MANU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include</t>
   </si>
 </sst>
 </file>
@@ -100,7 +159,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -124,17 +183,23 @@
       <family val="0"/>
     </font>
     <font>
-      <b val="true"/>
-      <sz val="14"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
+      <b val="true"/>
+      <sz val="9"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -153,7 +218,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -162,17 +227,10 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
+      <left style="hair"/>
+      <right style="hair"/>
+      <top style="hair"/>
+      <bottom style="hair"/>
       <diagonal/>
     </border>
   </borders>
@@ -206,36 +264,36 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -310,7 +368,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -321,38 +379,50 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="1:3"/>
+  <dimension ref="A1:Z7"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="4" ySplit="1" topLeftCell="E2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E10" activeCellId="0" sqref="E10"/>
+      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="11.0404858299595"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="10.412955465587"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="22.8502024291498"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="20.1740890688259"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="17.9757085020243"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="17.497975708502"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="21.4372469635628"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="18.2874493927126"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.5546558704453"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="20.6518218623482"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="24.9028340080972"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="17.0242914979757"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="22.5384615384615"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="22.2226720647773"/>
-    <col collapsed="false" hidden="false" max="1014" min="15" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1015" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.165991902834"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.42914979757085"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.331983805668"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6113360323887"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3967611336032"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1619433198381"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7246963562753"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9392712550607"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.3684210526316"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.95546558704453"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="25.6882591093117"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3765182186235"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="13.2631578947368"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.7894736842105"/>
+    <col collapsed="false" hidden="false" max="1015" min="27" style="1" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1016" style="2" width="9.1417004048583"/>
   </cols>
   <sheetData>
-    <row r="1" s="4" customFormat="true" ht="17.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
@@ -361,25 +431,25 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="E1" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="G1" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="J1" s="3" t="s">
         <v>9</v>
       </c>
       <c r="K1" s="3" t="s">
@@ -394,76 +464,254 @@
       <c r="N1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="3"/>
-      <c r="P1" s="3"/>
-      <c r="Q1" s="3"/>
-      <c r="R1" s="3"/>
-      <c r="AMA1" s="0"/>
-      <c r="AMB1" s="0"/>
-      <c r="AMC1" s="0"/>
-      <c r="AMD1" s="0"/>
-      <c r="AME1" s="0"/>
-      <c r="AMF1" s="0"/>
-      <c r="AMG1" s="0"/>
-      <c r="AMH1" s="0"/>
-      <c r="AMI1" s="0"/>
-      <c r="AMJ1" s="0"/>
+      <c r="O1" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" s="0"/>
     </row>
-    <row r="2" s="5" customFormat="true" ht="148.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D2" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="E2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F2" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="H2" s="7"/>
-      <c r="I2" s="7"/>
-      <c r="J2" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="K2" s="7"/>
-      <c r="L2" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="AMA2" s="0"/>
-      <c r="AMB2" s="0"/>
-      <c r="AMC2" s="0"/>
-      <c r="AMD2" s="0"/>
-      <c r="AME2" s="0"/>
-      <c r="AMF2" s="0"/>
-      <c r="AMG2" s="0"/>
-      <c r="AMH2" s="0"/>
-      <c r="AMI2" s="0"/>
-      <c r="AMJ2" s="0"/>
+    <row r="2" customFormat="false" ht="64.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H2" s="5"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="M2" s="4"/>
+      <c r="N2" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O2" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P2" s="7"/>
+      <c r="Z2" s="0"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="6"/>
-      <c r="D3" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="F3" s="5"/>
-      <c r="G3" s="8"/>
-      <c r="J3" s="7"/>
-      <c r="L3" s="5" t="s">
-        <v>19</v>
-      </c>
+      <c r="A3" s="4" t="s">
+        <v>32</v>
+      </c>
+      <c r="B3" s="4"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="E3" s="4"/>
+      <c r="F3" s="4"/>
+      <c r="G3" s="5"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+      <c r="J3" s="5"/>
+      <c r="K3" s="4"/>
+      <c r="L3" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M3" s="4"/>
+      <c r="N3" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O3" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P3" s="7"/>
+      <c r="Z3" s="0"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+      <c r="J4" s="4"/>
+      <c r="K4" s="4"/>
+      <c r="L4" s="4"/>
+      <c r="M4" s="4"/>
+      <c r="N4" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P4" s="7"/>
+      <c r="Z4" s="0"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+      <c r="J5" s="4"/>
+      <c r="K5" s="4"/>
+      <c r="L5" s="4"/>
+      <c r="M5" s="4"/>
+      <c r="N5" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O5" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P5" s="7"/>
+      <c r="Z5" s="0"/>
+    </row>
+    <row r="6" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M6" s="8" t="s">
+        <v>37</v>
+      </c>
+      <c r="N6" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O6" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P6" s="7"/>
+      <c r="Z6" s="0"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M7" s="4"/>
+      <c r="N7" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O7" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P7" s="7"/>
+      <c r="Z7" s="0"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-11454 CCJP KPI development
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="40">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -368,7 +368,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -386,39 +386,39 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="E1" activeCellId="0" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="K12" activeCellId="0" sqref="K12"/>
+      <selection pane="bottomRight" activeCell="C10" activeCellId="0" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.165991902834"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="26.3522267206478"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.331983805668"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6113360323887"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1619433198381"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7246963562753"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.95546558704453"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="25.6882591093117"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.7894736842105"/>
-    <col collapsed="false" hidden="false" max="1015" min="27" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1016" style="2" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.4251012145749"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.2105263157895"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9959514170041"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.4615384615385"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="13.2834008097166"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="16.9230769230769"/>
+    <col collapsed="false" hidden="false" max="1015" min="27" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1016" style="2" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -571,7 +571,9 @@
       <c r="A4" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B4" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C4" s="4" t="s">
         <v>34</v>
       </c>
@@ -598,7 +600,9 @@
       <c r="A5" s="4" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="4"/>
+      <c r="B5" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4"/>
@@ -619,7 +623,7 @@
       <c r="P5" s="7"/>
       <c r="Z5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="32.95" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="32.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="6" t="s">
         <v>36</v>
       </c>
@@ -672,7 +676,9 @@
       <c r="A7" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="C7" s="4" t="s">
         <v>26</v>
       </c>

</xml_diff>

<commit_message>
PROS-11454-CCJP POC KPI change for Tokyo stores
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -14,7 +14,7 @@
     <externalReference r:id="rId3"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$J$3</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="41">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -107,7 +107,7 @@
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
-    <t xml:space="preserve">Cold Teiban, Ambient Teiban</t>
+    <t xml:space="preserve">0001-Cold shelf, 0002-Ambient section</t>
   </si>
   <si>
     <t xml:space="preserve">include </t>
@@ -133,6 +133,9 @@
   </si>
   <si>
     <t xml:space="preserve">N/A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CCJP_POC_COUNT_BY_TASK</t>
   </si>
   <si>
     <t xml:space="preserve">CCJP_POC_SCORE_BY_TARGET</t>
@@ -375,7 +378,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -386,45 +389,34 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z7"/>
+  <dimension ref="A1:Z8"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="13" ySplit="1" topLeftCell="N2" activePane="bottomRight" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="topRight" activeCell="N1" activeCellId="0" sqref="N1"/>
       <selection pane="bottomLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I14" activeCellId="0" sqref="I14"/>
+      <selection pane="bottomRight" activeCell="B5" activeCellId="0" sqref="B5:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.7368421052632"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.2105263157895"/>
     <col collapsed="false" hidden="false" max="2" min="2" style="1" width="6.42914979757085"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="18.331983805668"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.6113360323887"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.3967611336032"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.1781376518219"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.1619433198381"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.7246963562753"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.3684210526316"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="9.95546558704453"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="16.7894736842105"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.3765182186235"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="13.2631578947368"/>
-    <col collapsed="false" hidden="false" max="1015" min="26" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1016" style="2" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="24.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="11.5708502024291"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.497975708502"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="10.8178137651822"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="12.1052631578947"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="14.5668016194332"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="10.1781376518219"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="17.0323886639676"/>
+    <col collapsed="false" hidden="false" max="25" min="14" style="1" width="13.3886639676113"/>
+    <col collapsed="false" hidden="false" max="1015" min="26" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1016" style="2" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -707,8 +699,8 @@
       <c r="Y5" s="4"/>
       <c r="Z5" s="0"/>
     </row>
-    <row r="6" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="6" t="s">
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
         <v>36</v>
       </c>
       <c r="B6" s="4" t="s">
@@ -744,8 +736,8 @@
       <c r="L6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="M6" s="8" t="s">
-        <v>37</v>
+      <c r="M6" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="N6" s="6" t="s">
         <v>30</v>
@@ -765,42 +757,46 @@
       <c r="Y6" s="4"/>
       <c r="Z6" s="0"/>
     </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M7" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="H7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J7" s="4"/>
-      <c r="K7" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L7" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="M7" s="4"/>
       <c r="N7" s="6" t="s">
         <v>30</v>
       </c>
@@ -819,6 +815,60 @@
       <c r="Y7" s="4"/>
       <c r="Z7" s="0"/>
     </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="F8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="I8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J8" s="4"/>
+      <c r="K8" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="M8" s="4"/>
+      <c r="N8" s="6" t="s">
+        <v>30</v>
+      </c>
+      <c r="O8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="4"/>
+      <c r="R8" s="4"/>
+      <c r="S8" s="4"/>
+      <c r="T8" s="4"/>
+      <c r="U8" s="4"/>
+      <c r="V8" s="4"/>
+      <c r="W8" s="4"/>
+      <c r="X8" s="4"/>
+      <c r="Y8" s="4"/>
+      <c r="Z8" s="0"/>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>

<commit_message>
PROS-14096 - CCJP FSOS SceneType KPIs
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="45">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -114,16 +114,16 @@
     <t xml:space="preserve">CCJP_FSOS_MANUF_BY_ALL_MANUF_IN_SCENE_TYPE</t>
   </si>
   <si>
+    <t xml:space="preserve">0001-Cold shelf, 0002-Ambient section</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exclude</t>
+  </si>
+  <si>
     <t xml:space="preserve">N/A</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0001-Cold shelf, 0002-Ambient section</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include </t>
-  </si>
-  <si>
-    <t xml:space="preserve">exclude</t>
   </si>
   <si>
     <t xml:space="preserve">Other, SSD, Coffee, Fruit Juice, 
@@ -136,13 +136,16 @@
     <t xml:space="preserve">Tokyo</t>
   </si>
   <si>
-    <t xml:space="preserve">CCJP_FSOS_MANUF_CAT_BY_ALL_MANU_CAT_IN_SCENE_TYPE</t>
+    <t xml:space="preserve">CCJP_FSOS_MANUF_CAT_BY_ALL_MANUF_CAT_IN_SCENE_TYPE</t>
   </si>
   <si>
     <t xml:space="preserve">Facings SOS</t>
   </si>
   <si>
     <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include </t>
   </si>
   <si>
     <t xml:space="preserve">CCJP_POC_COUNT_BY_STORE_AREA</t>
@@ -163,9 +166,6 @@
   </si>
   <si>
     <t xml:space="preserve">CCJP_UNIQUE_DIST_OWN_MANU</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include</t>
   </si>
 </sst>
 </file>
@@ -387,44 +387,44 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA10"/>
+  <dimension ref="A1:AA11"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F29" activeCellId="0" sqref="F29"/>
+      <selection pane="bottomLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="23.7368421052632"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="39.0607287449393"/>
-    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.09716599190283"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="21.8582995951417"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="10.9473684210526"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="9.84615384615385"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9.62753036437247"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.2753036437247"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.0607287449393"/>
-    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.40485829959514"/>
-    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.17004048583"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.4817813765182"/>
-    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.40485829959514"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="15.7975708502024"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.0485829959514"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="11.9392712550607"/>
-    <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.1417004048583"/>
-    <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.6356275303644"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.3846153846154"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.10526315789474"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.246963562753"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.4251012145749"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.4251012145749"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.10526315789474"/>
+    <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.10526315789474"/>
   </cols>
   <sheetData>
     <row r="1" s="4" customFormat="true" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -507,48 +507,46 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="0"/>
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="F2" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K2" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M2" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O2" s="2" t="s">
         <v>33</v>
@@ -559,48 +557,46 @@
       <c r="Q2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
-    <row r="3" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="C3" s="0"/>
+      <c r="D3" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="F3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K3" s="5" t="s">
         <v>32</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M3" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N3" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O3" s="2" t="s">
         <v>33</v>
@@ -611,30 +607,28 @@
       <c r="Q3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="55.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
         <v>36</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="C4" s="0"/>
+      <c r="D4" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="5" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="5" t="s">
-        <v>30</v>
-      </c>
       <c r="F4" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I4" s="5"/>
       <c r="J4" s="5"/>
@@ -643,10 +637,10 @@
       </c>
       <c r="L4" s="5"/>
       <c r="M4" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N4" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O4" s="2" t="s">
         <v>33</v>
@@ -665,18 +659,24 @@
         <v>37</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>28</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="D5" s="0"/>
       <c r="E5" s="5" t="s">
-        <v>30</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="F5" s="0"/>
+      <c r="G5" s="0"/>
       <c r="H5" s="5"/>
+      <c r="I5" s="0"/>
+      <c r="J5" s="0"/>
       <c r="K5" s="5"/>
+      <c r="L5" s="0"/>
       <c r="M5" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="N5" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O5" s="2" t="s">
         <v>33</v>
@@ -689,46 +689,46 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N6" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O6" s="2" t="s">
         <v>33</v>
@@ -741,46 +741,46 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N7" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O7" s="2" t="s">
         <v>33</v>
@@ -793,46 +793,46 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N8" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="O8" s="2" t="s">
         <v>33</v>
@@ -845,46 +845,46 @@
     </row>
     <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="I9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M9" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="O9" s="2" t="s">
         <v>33</v>
@@ -897,40 +897,40 @@
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="C10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D10" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D10" s="1" t="s">
+      <c r="E10" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E10" s="1" t="s">
-        <v>44</v>
-      </c>
       <c r="F10" s="1" t="s">
-        <v>44</v>
+        <v>29</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="M10" s="1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="O10" s="2" t="s">
         <v>33</v>
@@ -940,6 +940,11 @@
       </c>
       <c r="Q10" s="4"/>
       <c r="AA10" s="4"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="n">
+        <v>1</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -965,7 +970,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.1417004048583"/>
+    <col collapsed="false" hidden="false" max="1025" min="1" style="0" width="9.10526315789474"/>
   </cols>
   <sheetData/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>

<commit_message>
PROS-14222 - CCJP Bug Fix Channel 'N/A'
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="45">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -392,37 +392,37 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="F12" activeCellId="0" sqref="F12"/>
+      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="24.6356275303644"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="40.3846153846154"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.0647773279352"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.0283400809717"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.6032388663968"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.8178137651822"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.2834008097166"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.0688259109312"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.2834008097166"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.1740890688259"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.3198380566802"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.4251012145749"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.3198380566802"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3886639676113"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.5344129554656"/>
     <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.10526315789474"/>
   </cols>
@@ -651,16 +651,14 @@
       <c r="Q4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>31</v>
-      </c>
+      <c r="C5" s="0"/>
       <c r="D5" s="0"/>
       <c r="E5" s="5" t="s">
         <v>38</v>

</xml_diff>

<commit_message>
update template to calculate fsos for all regions
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="45">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -130,22 +130,22 @@
 NS Tea, Black Tea, Sports, Energy, Water, Vegetable Juice</t>
   </si>
   <si>
+    <t xml:space="preserve">CCJP_FSOS_MANUF_CAT_BY_ALL_MANUF_CAT_IN_SCENE_TYPE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Facings SOS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Availability</t>
+  </si>
+  <si>
+    <t xml:space="preserve">include </t>
+  </si>
+  <si>
     <t xml:space="preserve">address_city</t>
   </si>
   <si>
     <t xml:space="preserve">Tokyo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CCJP_FSOS_MANUF_CAT_BY_ALL_MANUF_CAT_IN_SCENE_TYPE</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Facings SOS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Availability</t>
-  </si>
-  <si>
-    <t xml:space="preserve">include </t>
   </si>
   <si>
     <t xml:space="preserve">CCJP_POC_COUNT_BY_STORE_AREA</t>
@@ -389,21 +389,20 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
+      <selection pane="bottomLeft" activeCell="S16" activeCellId="0" sqref="S16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.0647773279352"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.0283400809717"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2793522267206"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.3481781376518"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.8178137651822"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9230769230769"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="10.3886639676113"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="1" width="10.2834008097166"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.4251012145749"/>
@@ -411,18 +410,18 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.5344129554656"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.5344129554656"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.6396761133603"/>
     <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.10526315789474"/>
   </cols>
@@ -548,12 +547,8 @@
       <c r="N2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P2" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="O2" s="2"/>
+      <c r="P2" s="2"/>
       <c r="Q2" s="4"/>
       <c r="AA2" s="4"/>
     </row>
@@ -562,7 +557,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="0"/>
       <c r="D3" s="1" t="s">
@@ -598,21 +593,17 @@
       <c r="N3" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
       <c r="Q3" s="4"/>
       <c r="AA3" s="4"/>
     </row>
     <row r="4" customFormat="false" ht="55.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="0"/>
       <c r="D4" s="1" t="s">
@@ -642,26 +633,22 @@
       <c r="N4" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O4" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="P4" s="2" t="s">
-        <v>34</v>
-      </c>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
       <c r="Q4" s="4"/>
       <c r="AA4" s="4"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C5" s="0"/>
       <c r="D5" s="0"/>
       <c r="E5" s="5" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F5" s="0"/>
       <c r="G5" s="0"/>
@@ -677,10 +664,10 @@
         <v>31</v>
       </c>
       <c r="O5" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P5" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q5" s="4"/>
       <c r="AA5" s="4"/>
@@ -729,10 +716,10 @@
         <v>31</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q6" s="4"/>
       <c r="AA6" s="4"/>
@@ -781,10 +768,10 @@
         <v>31</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P7" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q7" s="4"/>
       <c r="AA7" s="4"/>
@@ -833,10 +820,10 @@
         <v>31</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q8" s="4"/>
       <c r="AA8" s="4"/>
@@ -885,10 +872,10 @@
         <v>43</v>
       </c>
       <c r="O9" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q9" s="4"/>
       <c r="AA9" s="4"/>
@@ -931,10 +918,10 @@
         <v>30</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="Q10" s="4"/>
       <c r="AA10" s="4"/>

</xml_diff>

<commit_message>
remove tokyo from all kpis
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -15,7 +15,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$K$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="43">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -140,12 +140,6 @@
   </si>
   <si>
     <t xml:space="preserve">include </t>
-  </si>
-  <si>
-    <t xml:space="preserve">address_city</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tokyo</t>
   </si>
   <si>
     <t xml:space="preserve">CCJP_POC_COUNT_BY_STORE_AREA</t>
@@ -376,7 +370,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -392,15 +386,15 @@
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="S16" activeCellId="0" sqref="S16"/>
+      <selection pane="bottomLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.2793522267206"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.3481781376518"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.4939271255061"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.668016194332"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="22.9230769230769"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.0323886639676"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.3886639676113"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
@@ -410,18 +404,18 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.6396761133603"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.6396761133603"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.748987854251"/>
     <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.10526315789474"/>
   </cols>
@@ -663,21 +657,17 @@
       <c r="N5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O5" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P5" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="O5" s="2"/>
+      <c r="P5" s="2"/>
       <c r="Q5" s="4"/>
       <c r="AA5" s="4"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>31</v>
@@ -715,21 +705,17 @@
       <c r="N6" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O6" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P6" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="O6" s="2"/>
+      <c r="P6" s="2"/>
       <c r="Q6" s="4"/>
       <c r="AA6" s="4"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>31</v>
@@ -767,21 +753,17 @@
       <c r="N7" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O7" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P7" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="O7" s="2"/>
+      <c r="P7" s="2"/>
       <c r="Q7" s="4"/>
       <c r="AA7" s="4"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>31</v>
@@ -819,21 +801,17 @@
       <c r="N8" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="O8" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P8" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="O8" s="2"/>
+      <c r="P8" s="2"/>
       <c r="Q8" s="4"/>
       <c r="AA8" s="4"/>
     </row>
-    <row r="9" customFormat="false" ht="28.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="28.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>31</v>
@@ -869,23 +847,19 @@
         <v>31</v>
       </c>
       <c r="N9" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="O9" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P9" s="2" t="s">
-        <v>38</v>
-      </c>
+        <v>41</v>
+      </c>
+      <c r="O9" s="2"/>
+      <c r="P9" s="2"/>
       <c r="Q9" s="4"/>
       <c r="AA9" s="4"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>31</v>
@@ -917,12 +891,8 @@
       <c r="M10" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="O10" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P10" s="2" t="s">
-        <v>38</v>
-      </c>
+      <c r="O10" s="2"/>
+      <c r="P10" s="2"/>
       <c r="Q10" s="4"/>
       <c r="AA10" s="4"/>
     </row>

</xml_diff>

<commit_message>
[PROS-1480] Removal of Hypens in scene type
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -15,7 +15,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$K$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -114,7 +114,7 @@
     <t xml:space="preserve">CCJP_FSOS_MANUF_BY_ALL_MANUF_IN_SCENE_TYPE</t>
   </si>
   <si>
-    <t xml:space="preserve">0001-Cold shelf, 0002-Ambient section</t>
+    <t xml:space="preserve">0001 Cold shelf, 0002 Ambient section</t>
   </si>
   <si>
     <t xml:space="preserve">include</t>
@@ -370,7 +370,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -383,39 +383,39 @@
   </sheetPr>
   <dimension ref="A1:AA11"/>
   <sheetViews>
-    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="H1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="topLeft" activeCell="H1" activeCellId="0" sqref="H1"/>
-      <selection pane="bottomLeft" activeCell="P19" activeCellId="0" sqref="P19"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.4939271255061"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.668016194332"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6032388663968"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.9919028340081"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.0323886639676"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1376518218623"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
-    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.3886639676113"/>
+    <col collapsed="false" hidden="false" max="9" min="9" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="10" min="10" style="1" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="11" min="11" style="1" width="11.246963562753"/>
-    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.497975708502"/>
+    <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.4251012145749"/>
-    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.748987854251"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.748987854251"/>
+    <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.497975708502"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.9595141700405"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.8542510121458"/>
     <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.10526315789474"/>
   </cols>
@@ -919,7 +919,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update to scene kpi results
</commit_message>
<xml_diff>
--- a/Projects/CCJP/Data/setup.xlsx
+++ b/Projects/CCJP/Data/setup.xlsx
@@ -15,7 +15,7 @@
     <externalReference r:id="rId4"/>
   </externalReferences>
   <definedNames>
-    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[2]Set_up!$A$90:$A$124</definedName>
+    <definedName function="false" hidden="false" name="Validation_List" vbProcedure="false">[1]Set_up!$A$90:$A$124</definedName>
     <definedName function="false" hidden="false" localSheetId="0" name="_xlnm._FilterDatabase" vbProcedure="false">'Functional KPIs'!$A$1:$K$5</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="148" uniqueCount="44">
   <si>
     <t xml:space="preserve">KPI Type</t>
   </si>
@@ -160,6 +160,9 @@
   </si>
   <si>
     <t xml:space="preserve">CCJP_UNIQUE_DIST_OWN_MANU</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FACINGS_OF_SKU_POSM_IN_CELL</t>
   </si>
 </sst>
 </file>
@@ -370,7 +373,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/externalLinks/externalLink2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
 <externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
 </externalLink>
@@ -381,20 +384,20 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AA11"/>
+  <dimension ref="A1:AA12"/>
   <sheetViews>
     <sheetView windowProtection="true" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="N2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.6032388663968"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="41.9919028340081"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="25.8137651821862"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="42.6315789473684"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="6.10526315789474"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.1376518218623"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="23.3522267206478"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="11.0323886639676"/>
     <col collapsed="false" hidden="false" max="7" min="6" style="1" width="10.497975708502"/>
     <col collapsed="false" hidden="false" max="8" min="8" style="1" width="11.246963562753"/>
@@ -404,18 +407,18 @@
     <col collapsed="false" hidden="false" max="12" min="12" style="1" width="13.6032388663968"/>
     <col collapsed="false" hidden="false" max="13" min="13" style="1" width="9.4251012145749"/>
     <col collapsed="false" hidden="false" max="14" min="14" style="1" width="16.497975708502"/>
-    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="12.8542510121458"/>
-    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="12.9595141700405"/>
-    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="12.8542510121458"/>
+    <col collapsed="false" hidden="false" max="15" min="15" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="16" min="16" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="17" min="17" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="18" min="18" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="19" min="19" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="20" min="20" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="21" min="21" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="22" min="22" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="23" min="23" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="24" min="24" style="1" width="13.0688259109312"/>
+    <col collapsed="false" hidden="false" max="25" min="25" style="1" width="13.1740890688259"/>
+    <col collapsed="false" hidden="false" max="26" min="26" style="1" width="13.0688259109312"/>
     <col collapsed="false" hidden="false" max="1016" min="27" style="1" width="9.10526315789474"/>
     <col collapsed="false" hidden="false" max="1025" min="1017" style="2" width="9.10526315789474"/>
   </cols>
@@ -885,6 +888,7 @@
       <c r="J10" s="1" t="s">
         <v>31</v>
       </c>
+      <c r="K10" s="0"/>
       <c r="L10" s="1" t="s">
         <v>31</v>
       </c>
@@ -897,7 +901,52 @@
       <c r="AA10" s="4"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="1" t="n">
+      <c r="A11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="O11" s="2"/>
+      <c r="P11" s="2"/>
+      <c r="Q11" s="4"/>
+      <c r="AA11" s="4"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>